<commit_message>
added pdf to excel
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -403,11 +403,11 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="60.83203125" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -435,10 +435,10 @@
         <v>Deposit</v>
       </c>
       <c r="B2" t="str">
-        <v>Deposit Refer: 130012345</v>
+        <v>DepositRef Nbr: 130012345</v>
       </c>
       <c r="C2" t="str">
-        <v>June 5, 2003</v>
+        <v>05-15</v>
       </c>
       <c r="D2">
         <v>3615.08</v>
@@ -447,7 +447,7 @@
         <v>USD</v>
       </c>
       <c r="F2" t="str">
-        <v>Income</v>
+        <v>Deposits &amp; Other Credits</v>
       </c>
     </row>
     <row r="3">
@@ -455,30 +455,30 @@
         <v>ATM Withdrawal</v>
       </c>
       <c r="B3" t="str">
-        <v>ATM Withdrawal 1000 Walnut St</v>
+        <v>ATM Withdrawal 1000 Walnut St M119 Kansas City MO 00005678</v>
       </c>
       <c r="C3" t="str">
-        <v>May 18, 2003</v>
+        <v>05-18</v>
       </c>
       <c r="D3">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="E3" t="str">
         <v>USD</v>
       </c>
       <c r="F3" t="str">
-        <v>Expense</v>
+        <v>ATM Withdrawals &amp; Debits</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Check Payment</v>
+        <v>Check Paid</v>
       </c>
       <c r="B4" t="str">
         <v>Check Number: 1001</v>
       </c>
       <c r="C4" t="str">
-        <v>May 12, 2003</v>
+        <v>05-12</v>
       </c>
       <c r="D4">
         <v>75</v>
@@ -487,38 +487,38 @@
         <v>USD</v>
       </c>
       <c r="F4" t="str">
-        <v>Expense</v>
+        <v>Checks Paid</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Check Payment</v>
+        <v>Check Paid</v>
       </c>
       <c r="B5" t="str">
         <v>Check Number: 1002</v>
       </c>
       <c r="C5" t="str">
-        <v>May 18, 2003</v>
+        <v>05-18</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>230</v>
       </c>
       <c r="E5" t="str">
         <v>USD</v>
       </c>
       <c r="F5" t="str">
-        <v>Expense</v>
+        <v>Checks Paid</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Check Payment</v>
+        <v>Check Paid</v>
       </c>
       <c r="B6" t="str">
         <v>Check Number: 1003</v>
       </c>
       <c r="C6" t="str">
-        <v>May 24, 2003</v>
+        <v>05-24</v>
       </c>
       <c r="D6">
         <v>200</v>
@@ -527,7 +527,7 @@
         <v>USD</v>
       </c>
       <c r="F6" t="str">
-        <v>Expense</v>
+        <v>Checks Paid</v>
       </c>
     </row>
   </sheetData>

</xml_diff>